<commit_message>
doc (Conception): Add MCD, MPD, Data Dictionnary
</commit_message>
<xml_diff>
--- a/conception/Champs_SGPC.xlsx
+++ b/conception/Champs_SGPC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.masson\Documents\SGPC\conception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v.masson\Documents\Projets de Stage\SGPC\conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -858,9 +858,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -870,58 +867,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,6 +899,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1232,7 +1232,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1241,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1284,7 +1284,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
   <sheetData>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="28" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1525,176 +1525,176 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="L1" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="P1" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="28" t="s">
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="28" t="s">
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="32" t="s">
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="AM1" s="34" t="s">
+      <c r="AM1" s="39" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="22" t="s">
+      <c r="A2" s="34"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="22" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="30" t="s">
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="U2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="W2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="X2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Y2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="AB2" s="30" t="s">
+      <c r="AB2" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="AC2" s="16" t="s">
+      <c r="AC2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="AD2" s="16" t="s">
+      <c r="AD2" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="AE2" s="16" t="s">
+      <c r="AE2" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="AF2" s="37" t="s">
+      <c r="AF2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="AG2" s="37" t="s">
+      <c r="AG2" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="AH2" s="37" t="s">
+      <c r="AH2" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="AI2" s="37" t="s">
+      <c r="AI2" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="AJ2" s="37" t="s">
+      <c r="AJ2" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="AK2" s="31" t="s">
+      <c r="AK2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="35"/>
+      <c r="AL2" s="42"/>
+      <c r="AM2" s="40"/>
     </row>
     <row r="3" spans="1:39" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1752,6 +1752,7 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="17">
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="U1:AA1"/>
@@ -1768,7 +1769,6 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="L1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1790,22 +1790,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1814,7 +1814,7 @@
       <c r="B2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="14"/>
@@ -1834,7 +1834,7 @@
       <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="25" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="13"/>
@@ -1874,7 +1874,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1914,7 +1914,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1947,13 +1947,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="30" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1981,7 +1981,7 @@
   <sheetData>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2021,7 +2021,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2059,7 +2059,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>